<commit_message>
corrected inverted upper/lower boundary for methanotrophic source
</commit_message>
<xml_diff>
--- a/artifacts/d13C_endmember_boundaries.xlsx
+++ b/artifacts/d13C_endmember_boundaries.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinekeller/Desktop/Keller_manu_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinekeller/Desktop/cascadia-margin-lipids/artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4639FE3D-4FC6-824B-97F3-E3981A0A5699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760F4E44-057F-5B45-B324-17AF1CAEC87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6380" yWindow="4500" windowWidth="26840" windowHeight="15940" xr2:uid="{CD2C46B5-BB4D-6940-A409-5598484EB2DE}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,10 +473,10 @@
         <v>2</v>
       </c>
       <c r="B3">
+        <v>-120</v>
+      </c>
+      <c r="C3">
         <v>-40</v>
-      </c>
-      <c r="C3">
-        <v>-120</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated d13C of benthic non-methane cycling endmember
</commit_message>
<xml_diff>
--- a/artifacts/d13C_endmember_boundaries.xlsx
+++ b/artifacts/d13C_endmember_boundaries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinekeller/Desktop/cascadia-margin-lipids/artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760F4E44-057F-5B45-B324-17AF1CAEC87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0CAE17-01DC-7F4D-892B-D02E50DCA5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6380" yWindow="4500" windowWidth="26840" windowHeight="15940" xr2:uid="{CD2C46B5-BB4D-6940-A409-5598484EB2DE}"/>
   </bookViews>
@@ -44,16 +44,16 @@
     <t>planktonic</t>
   </si>
   <si>
-    <t>methanotrophic</t>
-  </si>
-  <si>
-    <t>benthic</t>
-  </si>
-  <si>
     <t>Lower boundary</t>
   </si>
   <si>
     <t>Upper boudndary</t>
+  </si>
+  <si>
+    <t>benthic-methane cycling</t>
+  </si>
+  <si>
+    <t>benthic-non-methane cycling</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,10 +451,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -470,7 +470,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>-120</v>
@@ -481,13 +481,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>-34</v>
+        <v>-30</v>
       </c>
       <c r="C4">
-        <v>-24</v>
+        <v>-22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>